<commit_message>
12/11/2023 Complete the table and PowerPoint presentation
</commit_message>
<xml_diff>
--- a/Mikhail Bandurist Transistors/MoS2_samples.xlsx
+++ b/Mikhail Bandurist Transistors/MoS2_samples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e57f55479541be46/dottorato/LAUREANDI/Mikhail Bandurist/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Master Thesis\Mikhail Bandurist Transistors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB40FAE5-8C66-458E-A6B3-8D5CC20FAB53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65081B6C-2F6B-4253-B02C-97BC3BA71EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10650" windowHeight="12075" xr2:uid="{C9E8B9CF-8318-4199-AA93-CF4BA01BF75A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9E8B9CF-8318-4199-AA93-CF4BA01BF75A}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="72">
   <si>
     <t>batch</t>
   </si>
@@ -60,20 +60,218 @@
     <t>Sensitivity</t>
   </si>
   <si>
-    <t>MoS2 thickness</t>
-  </si>
-  <si>
     <t>Measurements</t>
   </si>
   <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.5±0.5 </t>
+  </si>
+  <si>
+    <t>MoS2 thickness (nm)</t>
+  </si>
+  <si>
+    <t>5.4±0.7</t>
+  </si>
+  <si>
+    <t>6.0±0.6</t>
+  </si>
+  <si>
+    <t>2.6±0.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.9±0.7 </t>
+  </si>
+  <si>
+    <t>trfSat (VDrain=1V), 
+trfLin (VDrain=0.1V), 
+output</t>
+  </si>
+  <si>
+    <t>trfSat (VDrain=1V), 
+trfLin (VDrain=0.05V), 
+output</t>
+  </si>
+  <si>
+    <t>Output curves go up</t>
+  </si>
+  <si>
+    <t>Output curves are almost linear</t>
+  </si>
+  <si>
+    <t>Small hysteresis</t>
+  </si>
+  <si>
+    <t>Small hysteresis,
+good output,
+trfLin starts from 20 V</t>
+  </si>
+  <si>
+    <t>NO SENSE, bad connection?</t>
+  </si>
+  <si>
+    <t>2.4±0.3</t>
+  </si>
+  <si>
+    <t>trfSat (VDrain=1V), 
+trfLin (VDrain=0.08V), 
+output</t>
+  </si>
+  <si>
+    <t>8.9±0.9</t>
+  </si>
+  <si>
+    <t>5.8±0.9</t>
+  </si>
+  <si>
+    <t>2.8±0.4</t>
+  </si>
+  <si>
+    <t>3.1±0.5</t>
+  </si>
+  <si>
+    <t>trfSat (VDrain=1V),
+output</t>
+  </si>
+  <si>
+    <t>Bad connection</t>
+  </si>
+  <si>
+    <t>trfSat (VDrain=1V), 
+trfLin (VDrain=0.2V), 
+output</t>
+  </si>
+  <si>
+    <t>Output is linear</t>
+  </si>
+  <si>
+    <t>trfSat (VDrain=1V)</t>
+  </si>
+  <si>
+    <t>IDrain is 0, bad connection</t>
+  </si>
+  <si>
+    <t>8.3±0.9</t>
+  </si>
+  <si>
+    <t>10.8±0.6</t>
+  </si>
+  <si>
+    <t>6.3±0.6</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>trfSat (VDrain=1V),  
+output</t>
+  </si>
+  <si>
+    <t>IDrain is picoAmps, 
+the contact not stable</t>
+  </si>
+  <si>
+    <t>Good results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.8±0.4 </t>
+  </si>
+  <si>
+    <t>3.8±0.4</t>
+  </si>
+  <si>
+    <t>5.7±0.3</t>
+  </si>
+  <si>
+    <t>No current</t>
+  </si>
+  <si>
+    <t>6.2±0.6</t>
+  </si>
+  <si>
+    <t>trfSat (VDrain=1V),
+trfLin(VDrain=0.1V),
+output</t>
+  </si>
+  <si>
+    <t>7.8±0.7</t>
+  </si>
+  <si>
+    <t>10.8±1.4</t>
+  </si>
+  <si>
+    <t>trfSat (VDrain=1V),
+output,
+trfLin (VDrain=0.2V)</t>
+  </si>
+  <si>
+    <t>At trfSat IDrain is microAmps, the plot is weird, bad connection?</t>
+  </si>
+  <si>
+    <t>3.9±0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.6±0.3 </t>
+  </si>
+  <si>
+    <t>8.7±0.4</t>
+  </si>
+  <si>
+    <t>8.0±0.5</t>
+  </si>
+  <si>
+    <t>9.4±0.5</t>
+  </si>
+  <si>
+    <t>trfSat (VDrain=1V),
+output,
+trfLin (VDrain=0.05V)</t>
+  </si>
+  <si>
+    <t>trfSat (VDrain=1V),
+output,
+trfLin (VDrain=0.1V)</t>
+  </si>
+  <si>
+    <t>3.6±0.4</t>
+  </si>
+  <si>
+    <t>9.2±0.8</t>
+  </si>
+  <si>
+    <t>4.8±0.6</t>
+  </si>
+  <si>
+    <t>3.3±03</t>
+  </si>
+  <si>
+    <t>4.8±0.3</t>
+  </si>
+  <si>
+    <t>trfSat (VDrain=1V),
+output,
+trfLin (VDrain=0.07V)</t>
+  </si>
+  <si>
+    <t>Output is linear, 
+could be leakage through insulator</t>
+  </si>
+  <si>
+    <t>Output is linear at higher VDrain</t>
+  </si>
+  <si>
+    <t>3.3±0.3</t>
+  </si>
+  <si>
+    <t>Hysteresis is big, output is almost linear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,8 +287,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,8 +317,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -112,19 +338,156 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCCC"/>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -137,7 +500,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -433,67 +796,1067 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879A3825-C697-4DF2-9C86-0190DF0EBED1}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
     <col min="8" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" customWidth="1"/>
-    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="20.5546875" customWidth="1"/>
+    <col min="14" max="14" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="11">
+        <v>2</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="16"/>
+      <c r="B8" s="12">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="16"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="16"/>
+      <c r="B10" s="12">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="1">
+        <v>4</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="12">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="1">
+        <v>5</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="16"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="16"/>
+      <c r="B19" s="12">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N19" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="16"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="1">
+        <v>4</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="16"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="1">
+        <v>5</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N21" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="16"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="16"/>
+      <c r="B23" s="12">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N23" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="16"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="4"/>
+    </row>
+    <row r="25" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="16"/>
+      <c r="B25" s="12">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N25" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="16"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="1">
+        <v>3</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N26" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="16"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="4"/>
+    </row>
+    <row r="28" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="16"/>
+      <c r="B28" s="12">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N28" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="16"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="1">
+        <v>2</v>
+      </c>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N29" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="16"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="1">
+        <v>3</v>
+      </c>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N30" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="16"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="1">
+        <v>5</v>
+      </c>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N31" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="16"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="1">
+        <v>6</v>
+      </c>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N32" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="16"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="4"/>
+    </row>
+    <row r="34" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="16"/>
+      <c r="B34" s="12">
+        <v>11</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N34" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="16"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="1">
+        <v>3</v>
+      </c>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N35" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="16"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="4"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="16"/>
+      <c r="B37" s="12">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N37" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="16"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="1">
+        <v>2</v>
+      </c>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N38" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="16"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="1">
+        <v>3</v>
+      </c>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="16"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="1">
+        <v>4</v>
+      </c>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N40" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" s="16"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="4"/>
+    </row>
+    <row r="42" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="16"/>
+      <c r="B42" s="12">
+        <v>14</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1</v>
+      </c>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N42" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="16"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="1">
+        <v>2</v>
+      </c>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N43" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="16"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="1">
+        <v>3</v>
+      </c>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N44" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="21"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="6">
+        <v>4</v>
+      </c>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="23"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="N45" s="24" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>